<commit_message>
some exercises is done like data validation.
</commit_message>
<xml_diff>
--- a/Kitap1.xlsx
+++ b/Kitap1.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YYY\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YYY\Desktop\BELGE\deneme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4391BF6-71C9-4FBB-8418-C02C5AE2796D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1200C5-FD82-40E1-A9DC-96D315EFF02B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{08DB501D-4982-4365-8FBA-E777E011E22F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sayfa1!$G$16:$J$24</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -56,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>YUNUS</t>
   </si>
@@ -95,6 +98,72 @@
   </si>
   <si>
     <t>BONUS</t>
+  </si>
+  <si>
+    <t>NEW ACTIVITY</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>SUB</t>
+  </si>
+  <si>
+    <t>MUL</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>NUM</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>SCORE</t>
+  </si>
+  <si>
+    <t>GRADES</t>
+  </si>
+  <si>
+    <t>JOHN</t>
+  </si>
+  <si>
+    <t>JONAS</t>
+  </si>
+  <si>
+    <t>JONATHAN</t>
+  </si>
+  <si>
+    <t>JACK</t>
+  </si>
+  <si>
+    <t>JIM</t>
+  </si>
+  <si>
+    <t>JANE</t>
+  </si>
+  <si>
+    <t>JULIE</t>
+  </si>
+  <si>
+    <t>GENDER</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>FEMALE</t>
+  </si>
+  <si>
+    <t>MALE Average</t>
+  </si>
+  <si>
+    <t>FEMALE Average</t>
+  </si>
+  <si>
+    <t>Grand Average</t>
   </si>
 </sst>
 </file>
@@ -104,7 +173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,8 +200,34 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,8 +282,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -196,11 +309,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -243,12 +371,40 @@
     <xf numFmtId="9" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,33 +719,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98FBD126-2347-4336-A110-3CC15E808C98}">
-  <dimension ref="A5:O27"/>
+  <dimension ref="A5:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.77734375" customWidth="1"/>
     <col min="6" max="6" width="17.109375" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" customWidth="1"/>
     <col min="9" max="9" width="13.77734375" customWidth="1"/>
-    <col min="10" max="10" width="11.21875" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" customWidth="1"/>
     <col min="14" max="14" width="17.5546875" customWidth="1"/>
     <col min="15" max="15" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
@@ -607,7 +763,7 @@
       <c r="F6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="18" t="s">
         <v>12</v>
       </c>
       <c r="K6" s="2"/>
@@ -629,7 +785,7 @@
         <f t="array" ref="F7:F10">(D7:D10)*(E7:E10)</f>
         <v>500</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="9">
@@ -647,7 +803,7 @@
       <c r="F8" s="5">
         <v>750</v>
       </c>
-      <c r="G8" s="20"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
@@ -665,7 +821,7 @@
       <c r="F9" s="5">
         <v>1350</v>
       </c>
-      <c r="G9" s="20"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="9">
@@ -683,7 +839,7 @@
       <c r="F10" s="5">
         <v>300</v>
       </c>
-      <c r="G10" s="20"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
@@ -702,7 +858,7 @@
         <f>AVERAGE(F7:F10)</f>
         <v>725</v>
       </c>
-      <c r="G11" s="21"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
@@ -721,30 +877,242 @@
         <f>MAX(F7:F10)</f>
         <v>1350</v>
       </c>
-      <c r="G12" s="21"/>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E13" s="1"/>
     </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G15" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+    </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E17" s="7"/>
-    </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="K27">
+      <c r="B16" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="G16" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="B17" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="23">
+        <v>2</v>
+      </c>
+      <c r="D17" s="23">
+        <v>3</v>
+      </c>
+      <c r="E17" s="24">
+        <f>C17+D17</f>
+        <v>5</v>
+      </c>
+      <c r="G17" s="30">
+        <v>1</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="27">
+        <v>20</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="B18" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="23">
+        <v>4</v>
+      </c>
+      <c r="D18" s="23">
+        <v>1</v>
+      </c>
+      <c r="E18" s="24">
+        <f>C18-D18</f>
+        <v>3</v>
+      </c>
+      <c r="G18" s="30">
+        <v>2</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="27">
+        <v>100</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="B19" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="23">
+        <v>8</v>
+      </c>
+      <c r="D19" s="23">
+        <v>7</v>
+      </c>
+      <c r="E19" s="24">
+        <f>C19*D19</f>
+        <v>56</v>
+      </c>
+      <c r="G19" s="30">
+        <v>3</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="27">
+        <v>80</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="B20" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="23">
+        <v>9</v>
+      </c>
+      <c r="D20" s="23">
+        <v>3</v>
+      </c>
+      <c r="E20" s="24">
+        <f>C20/D20</f>
+        <v>3</v>
+      </c>
+      <c r="G20" s="30">
+        <v>4</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="27">
+        <v>50</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="G21" s="30">
+        <v>5</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" s="27">
+        <v>35</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="G22" s="30"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27">
+        <f>SUBTOTAL(1,I17:I21)</f>
+        <v>57</v>
+      </c>
+      <c r="J22" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="G23" s="30">
+        <v>6</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" s="28">
+        <v>62</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="G24" s="30">
+        <v>7</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="28">
+        <v>89</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="G25" s="30"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28">
+        <f>SUBTOTAL(1,I23:I24)</f>
+        <v>75.5</v>
+      </c>
+      <c r="J25" s="31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G26" s="30"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28">
+        <f>SUBTOTAL(1,I17:I24)</f>
+        <v>62.285714285714285</v>
+      </c>
+      <c r="J26" s="31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K30">
         <f>G8</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <autoFilter ref="G16:J24" xr:uid="{8BB34612-6440-4034-A7AC-41C7B7B77065}"/>
+  <mergeCells count="3">
     <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="G15:J15"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Outside range error" error="please enter between 0-100." sqref="I17 I18 I19 I20 I21" xr:uid="{0FBE9E85-5DA7-4FD3-BAB2-3A5B49BD4981}">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
Days of week table were added.
</commit_message>
<xml_diff>
--- a/Kitap1.xlsx
+++ b/Kitap1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YYY\Desktop\BELGE\deneme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1200C5-FD82-40E1-A9DC-96D315EFF02B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DA3714-68C4-424F-8A01-AE97F62930AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{08DB501D-4982-4365-8FBA-E777E011E22F}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>YUNUS</t>
   </si>
@@ -164,6 +164,33 @@
   </si>
   <si>
     <t>Grand Average</t>
+  </si>
+  <si>
+    <t>SITUATION</t>
+  </si>
+  <si>
+    <t>DAYS OF WEEK</t>
+  </si>
+  <si>
+    <t>MONDAY</t>
+  </si>
+  <si>
+    <t>TUESDAY</t>
+  </si>
+  <si>
+    <t>WEDNESDAY</t>
+  </si>
+  <si>
+    <t>THURSDAY</t>
+  </si>
+  <si>
+    <t>FRIDAY</t>
+  </si>
+  <si>
+    <t>SATURDAY</t>
+  </si>
+  <si>
+    <t>SUNDAY</t>
   </si>
 </sst>
 </file>
@@ -227,7 +254,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,6 +327,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -328,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -374,37 +407,41 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,33 +756,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98FBD126-2347-4336-A110-3CC15E808C98}">
-  <dimension ref="A5:O30"/>
+  <dimension ref="A5:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
     <col min="5" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="12.109375" customWidth="1"/>
     <col min="9" max="9" width="13.77734375" customWidth="1"/>
     <col min="10" max="10" width="18.109375" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
     <col min="14" max="14" width="17.5546875" customWidth="1"/>
     <col min="15" max="15" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
@@ -785,7 +825,10 @@
         <f t="array" ref="F7:F10">(D7:D10)*(E7:E10)</f>
         <v>500</v>
       </c>
-      <c r="G7" s="19"/>
+      <c r="G7" s="19" t="b">
+        <f>AND(F7&gt;550,E7&gt;20%)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="9">
@@ -803,7 +846,10 @@
       <c r="F8" s="5">
         <v>750</v>
       </c>
-      <c r="G8" s="19"/>
+      <c r="G8" s="19" t="b">
+        <f t="shared" ref="G8:G10" si="0">AND(F8&gt;550,E8&gt;20%)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
@@ -821,7 +867,10 @@
       <c r="F9" s="5">
         <v>1350</v>
       </c>
-      <c r="G9" s="19"/>
+      <c r="G9" s="19" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="9">
@@ -839,7 +888,10 @@
       <c r="F10" s="5">
         <v>300</v>
       </c>
-      <c r="G10" s="19"/>
+      <c r="G10" s="19" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
@@ -883,232 +935,323 @@
       <c r="E13" s="1"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="G16" s="26" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="G16" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="I16" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="24" t="s">
         <v>29</v>
       </c>
+      <c r="K16" s="24" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="17" spans="2:11" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="22">
         <v>2</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="22">
         <v>3</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="23">
         <f>C17+D17</f>
         <v>5</v>
       </c>
-      <c r="G17" s="30">
+      <c r="G17" s="27">
         <v>1</v>
       </c>
-      <c r="H17" s="27" t="s">
+      <c r="H17" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="27">
+      <c r="I17" s="25">
         <v>20</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="K17" t="str">
+        <f>IF(I17&gt;70,"PASSED","FAILED")</f>
+        <v>FAILED</v>
+      </c>
     </row>
     <row r="18" spans="2:11" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="23">
+      <c r="C18" s="22">
         <v>4</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="22">
         <v>1</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="23">
         <f>C18-D18</f>
         <v>3</v>
       </c>
-      <c r="G18" s="30">
+      <c r="G18" s="27">
         <v>2</v>
       </c>
-      <c r="H18" s="27" t="s">
+      <c r="H18" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="27">
+      <c r="I18" s="25">
         <v>100</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="K18" t="str">
+        <f t="shared" ref="K18:K24" si="1">IF(I18&gt;70,"PASSED","FAILED")</f>
+        <v>PASSED</v>
+      </c>
     </row>
     <row r="19" spans="2:11" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="23">
+      <c r="C19" s="22">
         <v>8</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="22">
         <v>7</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="23">
         <f>C19*D19</f>
         <v>56</v>
       </c>
-      <c r="G19" s="30">
+      <c r="G19" s="27">
         <v>3</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="H19" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="27">
+      <c r="I19" s="25">
         <v>80</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>PASSED</v>
+      </c>
     </row>
     <row r="20" spans="2:11" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="23">
+      <c r="C20" s="22">
         <v>9</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="22">
         <v>3</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="23">
         <f>C20/D20</f>
         <v>3</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="27">
         <v>4</v>
       </c>
-      <c r="H20" s="27" t="s">
+      <c r="H20" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="27">
+      <c r="I20" s="25">
         <v>50</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>FAILED</v>
+      </c>
     </row>
     <row r="21" spans="2:11" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="G21" s="30">
+      <c r="G21" s="27">
         <v>5</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="H21" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="I21" s="27">
+      <c r="I21" s="25">
         <v>35</v>
       </c>
       <c r="J21" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>FAILED</v>
+      </c>
     </row>
     <row r="22" spans="2:11" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="G22" s="30"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27">
+      <c r="G22" s="27"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25">
         <f>SUBTOTAL(1,I17:I21)</f>
         <v>57</v>
       </c>
-      <c r="J22" s="31" t="s">
+      <c r="J22" s="28" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" spans="2:11" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="G23" s="30">
+      <c r="G23" s="27">
         <v>6</v>
       </c>
-      <c r="H23" s="28" t="s">
+      <c r="H23" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I23" s="28">
+      <c r="I23" s="26">
         <v>62</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>FAILED</v>
+      </c>
     </row>
     <row r="24" spans="2:11" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="G24" s="30">
+      <c r="G24" s="27">
         <v>7</v>
       </c>
-      <c r="H24" s="28" t="s">
+      <c r="H24" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="28">
+      <c r="I24" s="26">
         <v>89</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>PASSED</v>
+      </c>
     </row>
     <row r="25" spans="2:11" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="G25" s="30"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28">
+      <c r="G25" s="27"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26">
         <f>SUBTOTAL(1,I23:I24)</f>
         <v>75.5</v>
       </c>
-      <c r="J25" s="31" t="s">
+      <c r="J25" s="28" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G26" s="30"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28">
+      <c r="G26" s="27"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26">
         <f>SUBTOTAL(1,I17:I24)</f>
         <v>62.285714285714285</v>
       </c>
-      <c r="J26" s="31" t="s">
+      <c r="J26" s="28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="K30">
-        <f>G8</f>
-        <v>0</v>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="G32" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="H32" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" t="str">
+        <f>IF(B32="SATURDAY","PARTY HARD",IF(B32="SUNDAY","TIME TO REST","WORK"))</f>
+        <v>WORK</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" ref="C33:H33" si="2">IF(C32="SATURDAY","PARTY HARD",IF(C32="SUNDAY","TIME TO REST","WORK"))</f>
+        <v>WORK</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="2"/>
+        <v>WORK</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="2"/>
+        <v>WORK</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="2"/>
+        <v>WORK</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="2"/>
+        <v>PARTY HARD</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="2"/>
+        <v>TIME TO REST</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="G16:J24" xr:uid="{8BB34612-6440-4034-A7AC-41C7B7B77065}"/>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B16:E16"/>
-    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="B31:H31"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Outside range error" error="please enter between 0-100." sqref="I17 I18 I19 I20 I21" xr:uid="{0FBE9E85-5DA7-4FD3-BAB2-3A5B49BD4981}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Outside range error" error="please enter between 0-100." sqref="I17:I21" xr:uid="{0FBE9E85-5DA7-4FD3-BAB2-3A5B49BD4981}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
xml file loaded to folder and excel.
</commit_message>
<xml_diff>
--- a/Kitap1.xlsx
+++ b/Kitap1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YYY\Desktop\BELGE\deneme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEAF2D1-EF2C-4300-A580-3501C1E71D92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0F20D8-DF85-4F02-9BB0-865237C325D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{08DB501D-4982-4365-8FBA-E777E011E22F}"/>
   </bookViews>
@@ -1664,6 +1664,284 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>salary calculator</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sayfa1!$C$7:$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>YUSUF</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>YUNUS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MERT</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ALİ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sayfa1!$F$7:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9B22-4F60-9511-1F4FAAD9DC8A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1744,6 +2022,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2731,6 +3049,525 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2803,16 +3640,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>899160</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>937260</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2832,6 +3669,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC1D2A76-62D4-4FF3-A231-CF92B29CA6DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3151,8 +4024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98FBD126-2347-4336-A110-3CC15E808C98}">
   <dimension ref="A5:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Normalızation func is added in kitap1.
</commit_message>
<xml_diff>
--- a/Kitap1.xlsx
+++ b/Kitap1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YYY\Desktop\BELGE\deneme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0F20D8-DF85-4F02-9BB0-865237C325D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D896958-4E4F-4735-AD01-E43FF13C1F3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{08DB501D-4982-4365-8FBA-E777E011E22F}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>YUNUS</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>PRINTERS</t>
+  </si>
+  <si>
+    <t>SUMIF=&gt;</t>
+  </si>
+  <si>
+    <t>SALES OF PRODUCT(NORMALIZATION)</t>
   </si>
 </sst>
 </file>
@@ -216,7 +222,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +270,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
@@ -383,9 +397,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -451,6 +464,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -463,12 +479,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1755,6 +1772,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-9431-4A0D-B592-228D044ADAF5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1770,6 +1792,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-9431-4A0D-B592-228D044ADAF5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1785,6 +1812,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-9431-4A0D-B592-228D044ADAF5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1800,6 +1832,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-9431-4A0D-B592-228D044ADAF5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -4022,10 +4059,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98FBD126-2347-4336-A110-3CC15E808C98}">
-  <dimension ref="A5:O36"/>
+  <dimension ref="A5:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -4040,223 +4077,229 @@
     <col min="10" max="10" width="18.109375" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
     <col min="14" max="14" width="17.5546875" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="2"/>
+    <col min="15" max="15" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="2"/>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>1</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>2500</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>0.2</v>
       </c>
-      <c r="F7" s="5" cm="1">
+      <c r="F7" s="4" cm="1">
         <f t="array" ref="F7:F10">(D7:D10)*(E7:E10)</f>
         <v>500</v>
       </c>
-      <c r="G7" s="19" t="b">
+      <c r="G7" s="18" t="b">
         <f>AND(F7&gt;550,E7&gt;20%)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>2</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>3000</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>0.25</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>750</v>
       </c>
-      <c r="G8" s="19" t="b">
+      <c r="G8" s="18" t="b">
         <f t="shared" ref="G8:G10" si="0">AND(F8&gt;550,E8&gt;20%)</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>3</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>4500</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>0.3</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>1350</v>
       </c>
-      <c r="G9" s="19" t="b">
+      <c r="G9" s="18" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>4</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>2000</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>0.15</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>300</v>
       </c>
-      <c r="G10" s="19" t="b">
+      <c r="G10" s="18" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12">
+      <c r="C11" s="10"/>
+      <c r="D11" s="11">
         <f>AVERAGE(D7:D10)</f>
         <v>3000</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
         <f>AVERAGE(E7:E10)</f>
         <v>0.22500000000000001</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <f>AVERAGE(F7:F10)</f>
         <v>725</v>
       </c>
-      <c r="G11" s="20"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16">
+      <c r="C12" s="14"/>
+      <c r="D12" s="15">
         <f>MAX(D7:D10)</f>
         <v>4500</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="16">
         <f>MAX(E7:E10)</f>
         <v>0.3</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="15">
         <f>MAX(F7:F10)</f>
         <v>1350</v>
       </c>
-      <c r="G12" s="20"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E13" s="1"/>
+      <c r="E13" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13">
+        <f>SUMIF(D7:D10,"&gt;=2500",F7:F10)</f>
+        <v>2600</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="30" t="s">
+      <c r="A16" s="2"/>
+      <c r="B16" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="G16" s="24" t="s">
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="G16" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I16" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="24" t="s">
+      <c r="J16" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="K16" s="24" t="s">
+      <c r="K16" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:14" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="21">
         <v>2</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="21">
         <v>3</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="22">
         <f>C17+D17</f>
         <v>5</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="26">
         <v>1</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="H17" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="24">
         <v>20</v>
       </c>
-      <c r="J17" s="7" t="s">
+      <c r="J17" s="6" t="s">
         <v>30</v>
       </c>
       <c r="K17" t="str">
@@ -4265,29 +4308,29 @@
       </c>
     </row>
     <row r="18" spans="2:14" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="21">
         <v>4</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="21">
         <v>1</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="22">
         <f>C18-D18</f>
         <v>3</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="26">
         <v>2</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="H18" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="24">
         <v>100</v>
       </c>
-      <c r="J18" s="7" t="s">
+      <c r="J18" s="6" t="s">
         <v>30</v>
       </c>
       <c r="K18" t="str">
@@ -4296,29 +4339,29 @@
       </c>
     </row>
     <row r="19" spans="2:14" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="21">
         <v>8</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="21">
         <v>7</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="22">
         <f>C19*D19</f>
         <v>56</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="26">
         <v>3</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I19" s="24">
         <v>80</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="J19" s="6" t="s">
         <v>30</v>
       </c>
       <c r="K19" t="str">
@@ -4327,29 +4370,29 @@
       </c>
     </row>
     <row r="20" spans="2:14" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="21">
         <v>9</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="21">
         <v>3</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="22">
         <f>C20/D20</f>
         <v>3</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="26">
         <v>4</v>
       </c>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="25">
+      <c r="I20" s="24">
         <v>50</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="J20" s="6" t="s">
         <v>30</v>
       </c>
       <c r="K20" t="str">
@@ -4358,16 +4401,16 @@
       </c>
     </row>
     <row r="21" spans="2:14" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="G21" s="27">
+      <c r="G21" s="26">
         <v>5</v>
       </c>
-      <c r="H21" s="25" t="s">
+      <c r="H21" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I21" s="24">
         <v>35</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="J21" s="6" t="s">
         <v>30</v>
       </c>
       <c r="K21" t="str">
@@ -4376,27 +4419,27 @@
       </c>
     </row>
     <row r="22" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="G22" s="27"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25">
+      <c r="G22" s="26"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24">
         <f>SUBTOTAL(1,I17:I21)</f>
         <v>57</v>
       </c>
-      <c r="J22" s="28" t="s">
+      <c r="J22" s="27" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" spans="2:14" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="G23" s="27">
+      <c r="G23" s="26">
         <v>6</v>
       </c>
-      <c r="H23" s="26" t="s">
+      <c r="H23" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="I23" s="26">
+      <c r="I23" s="25">
         <v>62</v>
       </c>
-      <c r="J23" s="7" t="s">
+      <c r="J23" s="6" t="s">
         <v>31</v>
       </c>
       <c r="K23" t="str">
@@ -4405,16 +4448,16 @@
       </c>
     </row>
     <row r="24" spans="2:14" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="G24" s="27">
+      <c r="G24" s="26">
         <v>7</v>
       </c>
-      <c r="H24" s="26" t="s">
+      <c r="H24" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="26">
+      <c r="I24" s="25">
         <v>89</v>
       </c>
-      <c r="J24" s="7" t="s">
+      <c r="J24" s="6" t="s">
         <v>31</v>
       </c>
       <c r="K24" t="str">
@@ -4423,78 +4466,78 @@
       </c>
     </row>
     <row r="25" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="G25" s="27"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26">
+      <c r="G25" s="26"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25">
         <f>SUBTOTAL(1,I23:I24)</f>
         <v>75.5</v>
       </c>
-      <c r="J25" s="28" t="s">
+      <c r="J25" s="27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="G26" s="27"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26">
+      <c r="G26" s="26"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25">
         <f>SUBTOTAL(1,I17:I24)</f>
         <v>62.285714285714285</v>
       </c>
-      <c r="J26" s="28" t="s">
+      <c r="J26" s="27" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="J31" s="34" t="s">
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="J31" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="K31" s="34"/>
-      <c r="L31" s="34"/>
-      <c r="M31" s="34"/>
-      <c r="N31" s="34"/>
+      <c r="K31" s="35"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="35"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="D32" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F32" s="33" t="s">
+      <c r="F32" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="G32" s="33" t="s">
+      <c r="G32" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="H32" s="33" t="s">
+      <c r="H32" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36">
+      <c r="J32" s="30"/>
+      <c r="K32" s="30">
         <v>2011</v>
       </c>
-      <c r="L32" s="36">
+      <c r="L32" s="30">
         <v>2012</v>
       </c>
-      <c r="M32" s="36">
+      <c r="M32" s="30">
         <v>2013</v>
       </c>
-      <c r="N32" s="36">
+      <c r="N32" s="30">
         <v>2014</v>
       </c>
     </row>
@@ -4527,7 +4570,7 @@
         <f t="shared" si="2"/>
         <v>TIME TO REST</v>
       </c>
-      <c r="J33" s="35" t="s">
+      <c r="J33" s="29" t="s">
         <v>46</v>
       </c>
       <c r="K33">
@@ -4544,7 +4587,7 @@
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="J34" s="35" t="s">
+      <c r="J34" s="29" t="s">
         <v>45</v>
       </c>
       <c r="K34">
@@ -4561,7 +4604,7 @@
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="J35" s="35" t="s">
+      <c r="J35" s="29" t="s">
         <v>47</v>
       </c>
       <c r="K35">
@@ -4578,7 +4621,7 @@
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="J36" s="35" t="s">
+      <c r="J36" s="29" t="s">
         <v>48</v>
       </c>
       <c r="K36">
@@ -4592,11 +4635,120 @@
       </c>
       <c r="N36">
         <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D41" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D42" s="30"/>
+      <c r="E42" s="30">
+        <v>2011</v>
+      </c>
+      <c r="F42" s="30">
+        <v>2012</v>
+      </c>
+      <c r="G42" s="30">
+        <v>2013</v>
+      </c>
+      <c r="H42" s="30">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D43" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" s="37">
+        <f>(K33-MIN(K$33:K$36))/(MAX(K$33:K$36)-MIN(K$33:K$36))*100</f>
+        <v>13.23529411764706</v>
+      </c>
+      <c r="F43" s="37">
+        <f t="shared" ref="F43:H47" si="3">(L33-MIN(L$33:L$36))/(MAX(L$33:L$36)-MIN(L$33:L$36))*100</f>
+        <v>4.7619047619047619</v>
+      </c>
+      <c r="G43" s="37">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H43" s="37">
+        <f t="shared" si="3"/>
+        <v>9.5238095238095237</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D44" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" s="37">
+        <f t="shared" ref="E44:E46" si="4">(K34-MIN(K$33:K$36))/(MAX(K$33:K$36)-MIN(K$33:K$36))*100</f>
+        <v>5.8823529411764701</v>
+      </c>
+      <c r="F44" s="37">
+        <f t="shared" si="3"/>
+        <v>22.222222222222221</v>
+      </c>
+      <c r="G44" s="37">
+        <f t="shared" si="3"/>
+        <v>52.112676056338024</v>
+      </c>
+      <c r="H44" s="37">
+        <f t="shared" si="3"/>
+        <v>21.428571428571427</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D45" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E45" s="37">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F45" s="37">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G45" s="37">
+        <f t="shared" si="3"/>
+        <v>14.084507042253522</v>
+      </c>
+      <c r="H45" s="37">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="D46" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E46" s="37">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="F46" s="37">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="G46" s="37">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="H46" s="37">
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="G16:J24" xr:uid="{8BB34612-6440-4034-A7AC-41C7B7B77065}"/>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="D41:H41"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="G15:K15"/>

</xml_diff>